<commit_message>
redirect to url issue resolved!
</commit_message>
<xml_diff>
--- a/poi-generated-file.xlsx
+++ b/poi-generated-file.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Client Manager Name</t>
   </si>
@@ -90,19 +90,13 @@
     <t>5-Aug</t>
   </si>
   <si>
-    <t xml:space="preserve">Client Call ( sancjit ) </t>
-  </si>
-  <si>
-    <t>12</t>
+    <t xml:space="preserve">Development ( 1 ) </t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>38</t>
+    <t>7</t>
   </si>
   <si>
     <t>Offshore Consultant's Project Manager's Name :dhananjayKumar@gmail.com</t>
@@ -1157,22 +1151,22 @@
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" s="9"/>
     </row>
@@ -1298,22 +1292,22 @@
         <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L18" s="10"/>
     </row>
@@ -1323,7 +1317,7 @@
       </c>
       <c r="C19" s="83"/>
       <c r="D19" s="84" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E19" s="84"/>
       <c r="F19" s="84"/>
@@ -1367,7 +1361,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
@@ -1413,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>

</xml_diff>

<commit_message>
"typeahead and description enlarged functionality"
</commit_message>
<xml_diff>
--- a/poi-generated-file.xlsx
+++ b/poi-generated-file.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Client Manager Name</t>
   </si>
@@ -90,19 +90,22 @@
     <t>19-Aug</t>
   </si>
   <si>
-    <t xml:space="preserve">Status Call ( s1 ) </t>
+    <t xml:space="preserve">q ( bvcvbcbbc ) </t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Offshore Consultant's Project Manager's Name :Vivek sharma</t>
-  </si>
-  <si>
-    <t>Omar</t>
+    <t>37</t>
+  </si>
+  <si>
+    <t>Offshore Consultant's Project Manager's Name :Tanuj Khaturia</t>
+  </si>
+  <si>
+    <t>Omar Colon</t>
   </si>
 </sst>
 </file>
@@ -1157,16 +1160,16 @@
         <v>22</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L9" s="9"/>
     </row>
@@ -1298,16 +1301,16 @@
         <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L18" s="10"/>
     </row>
@@ -1317,7 +1320,7 @@
       </c>
       <c r="C19" s="83"/>
       <c r="D19" s="84" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E19" s="84"/>
       <c r="F19" s="84"/>
@@ -1361,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
@@ -1407,7 +1410,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>

</xml_diff>